<commit_message>
master: Routing POC complete and started creating pages from the beginning.
</commit_message>
<xml_diff>
--- a/Misc Files/3.xlsx
+++ b/Misc Files/3.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b15c2d483f869a28/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\bangla-school-app\Misc Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{658CECE3-5C65-430D-BA74-E69818F01FC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EB38078-E855-4253-B4A0-1AEA1CDE23D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{7629C9F7-A4E1-4BBF-A988-E2BC0BBB0955}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>ট</t>
   </si>
@@ -144,6 +144,15 @@
   </si>
   <si>
     <t>ম</t>
+  </si>
+  <si>
+    <t>য</t>
+  </si>
+  <si>
+    <t>র</t>
+  </si>
+  <si>
+    <t>ল</t>
   </si>
 </sst>
 </file>
@@ -505,8 +514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{662B3F94-04A4-4B98-80BE-AF06FAC25752}">
   <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="46.2" x14ac:dyDescent="0.85"/>
@@ -522,25 +531,25 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E1" s="1">
         <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="H1" s="1">
         <v>16</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="K1" s="1">
         <v>24</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="N1" s="1">
         <v>32</v>
@@ -554,25 +563,25 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E2" s="1">
         <v>9</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="H2" s="1">
         <v>17</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="K2" s="1">
         <v>25</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="N2" s="1">
         <v>33</v>
@@ -586,25 +595,25 @@
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E3" s="1">
         <v>10</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H3" s="1">
         <v>18</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="K3" s="1">
         <v>26</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="N3" s="1">
         <v>34</v>
@@ -618,25 +627,25 @@
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E4" s="1">
         <v>11</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H4" s="1">
         <v>19</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="K4" s="1">
         <v>27</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="N4" s="1">
         <v>35</v>
@@ -650,25 +659,25 @@
         <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E5" s="1">
         <v>12</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H5" s="1">
         <v>20</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K5" s="1">
         <v>28</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="N5" s="1">
         <v>36</v>
@@ -676,80 +685,98 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.85">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="B6" s="1">
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E6" s="1">
         <v>13</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H6" s="1">
         <v>21</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="K6" s="1">
         <v>29</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N6" s="1">
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.85">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="B7" s="1">
         <v>6</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E7" s="1">
         <v>14</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H7" s="1">
         <v>22</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K7" s="1">
         <v>30</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N7" s="1">
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.85">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="B8" s="1">
         <v>7</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="E8" s="1">
         <v>15</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H8" s="1">
         <v>23</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="K8" s="1">
         <v>31</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N8" s="1">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>